<commit_message>
se suben archivos para eeff
</commit_message>
<xml_diff>
--- a/docs/demo/set-datos/configuracion-nota-7.xlsx
+++ b/docs/demo/set-datos/configuracion-nota-7.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="405" windowWidth="19800" windowHeight="9900"/>
+    <workbookView xWindow="330" yWindow="465" windowWidth="19800" windowHeight="9840"/>
   </bookViews>
   <sheets>
     <sheet name="Nota 7" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -60,41 +60,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,17 +80,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6E9EE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -121,35 +93,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,9 +408,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -470,103 +420,104 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>